<commit_message>
Changes biomarker "TP53" to "p53" label
</commit_message>
<xml_diff>
--- a/inst/extdata/biomarker_rules_enoc.xlsx
+++ b/inst/extdata/biomarker_rules_enoc.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hannahokada/Documents/GitHub/EDGEResearch - CA:TMATools/TMAtools/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{110153C4-3162-3A4A-A443-24AF1EAA5E81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{144E546F-DEAC-8946-B74D-8D2D5B49BAB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="translation" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="69">
   <si>
     <t>biomarker</t>
   </si>
@@ -225,6 +225,9 @@
   </si>
   <si>
     <t xml:space="preserve">subclonal </t>
+  </si>
+  <si>
+    <t>p53</t>
   </si>
 </sst>
 </file>
@@ -625,8 +628,8 @@
   </sheetPr>
   <dimension ref="A1:C124"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E133" sqref="E133"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -715,7 +718,7 @@
     </row>
     <row r="8" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>68</v>
       </c>
       <c r="B8" s="4">
         <v>0</v>
@@ -726,7 +729,7 @@
     </row>
     <row r="9" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>68</v>
       </c>
       <c r="B9" s="4">
         <v>1</v>
@@ -737,7 +740,7 @@
     </row>
     <row r="10" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>68</v>
       </c>
       <c r="B10" s="4">
         <v>2</v>
@@ -748,7 +751,7 @@
     </row>
     <row r="11" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>68</v>
       </c>
       <c r="B11" s="4">
         <v>3</v>
@@ -759,7 +762,7 @@
     </row>
     <row r="12" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>68</v>
       </c>
       <c r="B12" s="4">
         <v>4</v>
@@ -770,7 +773,7 @@
     </row>
     <row r="13" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>68</v>
       </c>
       <c r="B13" s="4">
         <v>5</v>
@@ -781,7 +784,7 @@
     </row>
     <row r="14" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>10</v>
+        <v>68</v>
       </c>
       <c r="B14" s="4">
         <v>8</v>
@@ -792,7 +795,7 @@
     </row>
     <row r="15" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>10</v>
+        <v>68</v>
       </c>
       <c r="B15" s="4">
         <v>9</v>
@@ -803,7 +806,7 @@
     </row>
     <row r="16" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>10</v>
+        <v>68</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>37</v>
@@ -814,7 +817,7 @@
     </row>
     <row r="17" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>10</v>
+        <v>68</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>11</v>
@@ -2001,6 +2004,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2012,7 +2016,7 @@
   </sheetPr>
   <dimension ref="A1:D57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="150" workbookViewId="0">
+    <sheetView zoomScale="80" workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added biomarkers to consolidation sheet
</commit_message>
<xml_diff>
--- a/inst/extdata/biomarker_rules_enoc.xlsx
+++ b/inst/extdata/biomarker_rules_enoc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hannahokada/Documents/GitHub/EDGEResearch - CA:TMATools/TMAtools/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{144E546F-DEAC-8946-B74D-8D2D5B49BAB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0F21FEA-5D8A-AE4E-AF36-FF183BFCFE54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16340" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="translation" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="66">
   <si>
     <t>biomarker</t>
   </si>
@@ -98,9 +98,6 @@
     <t>any;any</t>
   </si>
   <si>
-    <t>absent;retained</t>
-  </si>
-  <si>
     <t>retained</t>
   </si>
   <si>
@@ -113,18 +110,6 @@
     <t>nuclear</t>
   </si>
   <si>
-    <t>aaa;b</t>
-  </si>
-  <si>
-    <t>ab</t>
-  </si>
-  <si>
-    <t>aaa</t>
-  </si>
-  <si>
-    <t>a</t>
-  </si>
-  <si>
     <t>reduced</t>
   </si>
   <si>
@@ -228,6 +213,12 @@
   </si>
   <si>
     <t>p53</t>
+  </si>
+  <si>
+    <t xml:space="preserve">absent;retained </t>
+  </si>
+  <si>
+    <t>absent;reduced</t>
   </si>
 </sst>
 </file>
@@ -277,7 +268,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79998168889431442"/>
+        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -315,12 +306,12 @@
     <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="3" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -628,14 +619,14 @@
   </sheetPr>
   <dimension ref="A1:C124"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.83203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.83203125" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -644,10 +635,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -699,7 +690,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
@@ -718,7 +709,7 @@
     </row>
     <row r="8" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B8" s="4">
         <v>0</v>
@@ -729,7 +720,7 @@
     </row>
     <row r="9" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B9" s="4">
         <v>1</v>
@@ -740,7 +731,7 @@
     </row>
     <row r="10" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B10" s="4">
         <v>2</v>
@@ -751,7 +742,7 @@
     </row>
     <row r="11" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B11" s="4">
         <v>3</v>
@@ -762,7 +753,7 @@
     </row>
     <row r="12" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B12" s="4">
         <v>4</v>
@@ -773,7 +764,7 @@
     </row>
     <row r="13" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B13" s="4">
         <v>5</v>
@@ -784,7 +775,7 @@
     </row>
     <row r="14" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B14" s="4">
         <v>8</v>
@@ -795,7 +786,7 @@
     </row>
     <row r="15" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B15" s="4">
         <v>9</v>
@@ -806,10 +797,10 @@
     </row>
     <row r="16" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C16" t="s">
         <v>11</v>
@@ -817,7 +808,7 @@
     </row>
     <row r="17" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>11</v>
@@ -897,18 +888,18 @@
         <v>19</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C24" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>19</v>
       </c>
-      <c r="B25" s="6" t="s">
-        <v>38</v>
+      <c r="B25" s="5" t="s">
+        <v>33</v>
       </c>
       <c r="C25" t="s">
         <v>11</v>
@@ -933,7 +924,7 @@
         <v>1</v>
       </c>
       <c r="C27" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -944,7 +935,7 @@
         <v>2</v>
       </c>
       <c r="C28" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -955,7 +946,7 @@
         <v>3</v>
       </c>
       <c r="C29" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -977,7 +968,7 @@
         <v>5</v>
       </c>
       <c r="C31" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -996,7 +987,7 @@
         <v>23</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C33" t="s">
         <v>11</v>
@@ -1006,7 +997,7 @@
       <c r="A34" t="s">
         <v>23</v>
       </c>
-      <c r="B34" s="6" t="s">
+      <c r="B34" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C34" t="s">
@@ -1015,7 +1006,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B35" s="4">
         <v>0</v>
@@ -1026,7 +1017,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B36" s="4">
         <v>1</v>
@@ -1037,7 +1028,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B37" s="4">
         <v>2</v>
@@ -1048,7 +1039,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B38" s="4">
         <v>9</v>
@@ -1059,10 +1050,10 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C39" t="s">
         <v>11</v>
@@ -1070,7 +1061,7 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>11</v>
@@ -1081,7 +1072,7 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B41" s="4">
         <v>0</v>
@@ -1092,7 +1083,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B42" s="4">
         <v>1</v>
@@ -1103,7 +1094,7 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B43" s="4">
         <v>2</v>
@@ -1114,7 +1105,7 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B44" s="4">
         <v>9</v>
@@ -1125,10 +1116,10 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C45" t="s">
         <v>11</v>
@@ -1136,7 +1127,7 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>11</v>
@@ -1147,7 +1138,7 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B47" s="4">
         <v>0</v>
@@ -1158,7 +1149,7 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B48" s="4">
         <v>1</v>
@@ -1169,7 +1160,7 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B49" s="4">
         <v>2</v>
@@ -1180,7 +1171,7 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B50" s="4">
         <v>9</v>
@@ -1191,10 +1182,10 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C51" t="s">
         <v>11</v>
@@ -1202,7 +1193,7 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B52" s="3" t="s">
         <v>11</v>
@@ -1213,7 +1204,7 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B53" s="4">
         <v>0</v>
@@ -1224,7 +1215,7 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B54" s="4">
         <v>1</v>
@@ -1235,7 +1226,7 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B55" s="4">
         <v>2</v>
@@ -1246,7 +1237,7 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B56" s="4">
         <v>9</v>
@@ -1257,10 +1248,10 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C57" t="s">
         <v>11</v>
@@ -1268,7 +1259,7 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B58" s="3" t="s">
         <v>11</v>
@@ -1279,7 +1270,7 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B59" s="4">
         <v>0</v>
@@ -1290,7 +1281,7 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B60" s="4">
         <v>1</v>
@@ -1301,7 +1292,7 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B61" s="4">
         <v>2</v>
@@ -1312,7 +1303,7 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B62" s="4">
         <v>9</v>
@@ -1323,10 +1314,10 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C63" t="s">
         <v>11</v>
@@ -1334,7 +1325,7 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B64" s="3" t="s">
         <v>11</v>
@@ -1345,7 +1336,7 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B65" s="4">
         <v>0</v>
@@ -1356,7 +1347,7 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B66" s="4">
         <v>1</v>
@@ -1367,7 +1358,7 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B67" s="4">
         <v>2</v>
@@ -1378,7 +1369,7 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B68" s="4">
         <v>9</v>
@@ -1389,10 +1380,10 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C69" t="s">
         <v>11</v>
@@ -1400,7 +1391,7 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B70" s="3" t="s">
         <v>11</v>
@@ -1411,9 +1402,9 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>45</v>
-      </c>
-      <c r="B71" s="6">
+        <v>40</v>
+      </c>
+      <c r="B71" s="5">
         <v>0</v>
       </c>
       <c r="C71" t="s">
@@ -1422,54 +1413,54 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>45</v>
-      </c>
-      <c r="B72" s="6">
+        <v>40</v>
+      </c>
+      <c r="B72" s="5">
         <v>1</v>
       </c>
       <c r="C72" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>45</v>
-      </c>
-      <c r="B73" s="6">
+        <v>40</v>
+      </c>
+      <c r="B73" s="5">
         <v>2</v>
       </c>
       <c r="C73" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>45</v>
-      </c>
-      <c r="B74" s="6">
+        <v>40</v>
+      </c>
+      <c r="B74" s="5">
         <v>3</v>
       </c>
       <c r="C74" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>45</v>
-      </c>
-      <c r="B75" s="6">
+        <v>40</v>
+      </c>
+      <c r="B75" s="5">
         <v>9</v>
       </c>
       <c r="C75" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>45</v>
-      </c>
-      <c r="B76" s="6" t="s">
-        <v>37</v>
+        <v>40</v>
+      </c>
+      <c r="B76" s="5" t="s">
+        <v>32</v>
       </c>
       <c r="C76" t="s">
         <v>11</v>
@@ -1477,9 +1468,9 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>45</v>
-      </c>
-      <c r="B77" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B77" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C77" t="s">
@@ -1488,7 +1479,7 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B78" s="4">
         <v>0</v>
@@ -1499,7 +1490,7 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B79" s="4">
         <v>1</v>
@@ -1510,7 +1501,7 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B80" s="4">
         <v>2</v>
@@ -1521,7 +1512,7 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B81" s="4">
         <v>3</v>
@@ -1532,7 +1523,7 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B82" s="4">
         <v>8</v>
@@ -1543,7 +1534,7 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B83" s="4">
         <v>9</v>
@@ -1554,10 +1545,10 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C84" t="s">
         <v>11</v>
@@ -1565,18 +1556,18 @@
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C85" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B86" s="4">
         <v>0</v>
@@ -1587,7 +1578,7 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B87" s="4">
         <v>1</v>
@@ -1598,7 +1589,7 @@
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B88" s="4">
         <v>2</v>
@@ -1609,7 +1600,7 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B89" s="4">
         <v>3</v>
@@ -1620,7 +1611,7 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B90" s="4">
         <v>8</v>
@@ -1631,7 +1622,7 @@
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B91" s="4">
         <v>9</v>
@@ -1642,10 +1633,10 @@
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C92" t="s">
         <v>11</v>
@@ -1653,18 +1644,18 @@
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C93" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B94" s="4">
         <v>0</v>
@@ -1675,7 +1666,7 @@
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B95" s="4">
         <v>1</v>
@@ -1686,7 +1677,7 @@
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B96" s="4">
         <v>2</v>
@@ -1697,7 +1688,7 @@
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B97" s="4">
         <v>3</v>
@@ -1708,7 +1699,7 @@
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B98" s="4">
         <v>8</v>
@@ -1719,7 +1710,7 @@
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B99" s="4">
         <v>9</v>
@@ -1730,21 +1721,21 @@
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C100" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>51</v>
-      </c>
-      <c r="B101" s="6" t="s">
-        <v>38</v>
+        <v>46</v>
+      </c>
+      <c r="B101" s="5" t="s">
+        <v>33</v>
       </c>
       <c r="C101" t="s">
         <v>11</v>
@@ -1752,7 +1743,7 @@
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B102" s="4">
         <v>0</v>
@@ -1763,7 +1754,7 @@
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B103" s="4">
         <v>1</v>
@@ -1774,7 +1765,7 @@
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B104" s="4">
         <v>2</v>
@@ -1785,7 +1776,7 @@
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B105" s="4">
         <v>3</v>
@@ -1796,7 +1787,7 @@
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B106" s="4">
         <v>8</v>
@@ -1807,7 +1798,7 @@
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B107" s="4">
         <v>9</v>
@@ -1818,10 +1809,10 @@
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C108" t="s">
         <v>11</v>
@@ -1829,10 +1820,10 @@
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C109" t="s">
         <v>11</v>
@@ -1840,7 +1831,7 @@
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B110" s="4">
         <v>0</v>
@@ -1851,7 +1842,7 @@
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B111" s="4">
         <v>1</v>
@@ -1862,7 +1853,7 @@
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B112" s="4">
         <v>2</v>
@@ -1873,7 +1864,7 @@
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B113" s="4">
         <v>3</v>
@@ -1884,7 +1875,7 @@
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B114" s="4">
         <v>8</v>
@@ -1895,7 +1886,7 @@
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B115" s="4">
         <v>9</v>
@@ -1906,10 +1897,10 @@
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C116" t="s">
         <v>11</v>
@@ -1917,90 +1908,90 @@
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C117" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>54</v>
-      </c>
-      <c r="B118" s="6">
+        <v>49</v>
+      </c>
+      <c r="B118" s="5">
         <v>0</v>
       </c>
       <c r="C118" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>54</v>
-      </c>
-      <c r="B119" s="6">
+        <v>49</v>
+      </c>
+      <c r="B119" s="5">
         <v>1</v>
       </c>
       <c r="C119" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>54</v>
-      </c>
-      <c r="B120" s="6">
+        <v>49</v>
+      </c>
+      <c r="B120" s="5">
         <v>2</v>
       </c>
       <c r="C120" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>58</v>
-      </c>
-      <c r="B121" s="6">
+        <v>53</v>
+      </c>
+      <c r="B121" s="5">
         <v>3</v>
       </c>
       <c r="C121" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>58</v>
-      </c>
-      <c r="B122" s="6">
+        <v>53</v>
+      </c>
+      <c r="B122" s="5">
         <v>9</v>
       </c>
       <c r="C122" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>58</v>
-      </c>
-      <c r="B123" s="6" t="s">
-        <v>37</v>
+        <v>53</v>
+      </c>
+      <c r="B123" s="5" t="s">
+        <v>32</v>
       </c>
       <c r="C123" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>54</v>
-      </c>
-      <c r="B124" s="6" t="s">
-        <v>38</v>
+        <v>49</v>
+      </c>
+      <c r="B124" s="5" t="s">
+        <v>33</v>
       </c>
       <c r="C124" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -2016,14 +2007,14 @@
   </sheetPr>
   <dimension ref="A1:D57"/>
   <sheetViews>
-    <sheetView zoomScale="80" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="220" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.83203125" bestFit="1" customWidth="1"/>
   </cols>
@@ -2206,10 +2197,10 @@
         <v>23</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C14" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D14" t="s">
         <v>17</v>
@@ -2219,11 +2210,11 @@
       <c r="A15" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>24</v>
+      <c r="B15" s="8">
+        <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>25</v>
+        <v>65</v>
       </c>
       <c r="D15" t="s">
         <v>17</v>
@@ -2233,53 +2224,53 @@
       <c r="A16" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>5</v>
+      <c r="B16" s="8" t="s">
+        <v>24</v>
       </c>
       <c r="C16" t="s">
-        <v>20</v>
+        <v>64</v>
       </c>
       <c r="D16" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>23</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>5</v>
+      <c r="B17" s="8" t="s">
+        <v>26</v>
       </c>
       <c r="C17" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D17" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>23</v>
       </c>
-      <c r="B18" s="3" t="s">
-        <v>27</v>
+      <c r="B18" s="8" t="s">
+        <v>5</v>
       </c>
       <c r="C18" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D18" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>23</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C19" t="s">
         <v>27</v>
-      </c>
-      <c r="C19" t="s">
-        <v>29</v>
       </c>
       <c r="D19" t="s">
         <v>11</v>
@@ -2289,25 +2280,25 @@
       <c r="A20" t="s">
         <v>23</v>
       </c>
-      <c r="B20" s="4" t="s">
-        <v>24</v>
+      <c r="B20" s="8" t="s">
+        <v>55</v>
       </c>
       <c r="C20" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D20" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>23</v>
       </c>
-      <c r="B21" s="5">
-        <v>2</v>
+      <c r="B21" s="8" t="s">
+        <v>5</v>
       </c>
       <c r="C21" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D21" t="s">
         <v>33</v>
@@ -2321,12 +2312,12 @@
         <v>8</v>
       </c>
       <c r="D22" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>5</v>
@@ -2340,7 +2331,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>5</v>
@@ -2354,7 +2345,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>8</v>
@@ -2365,7 +2356,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>5</v>
@@ -2379,7 +2370,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>5</v>
@@ -2393,7 +2384,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>8</v>
@@ -2404,7 +2395,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>5</v>
@@ -2418,7 +2409,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>5</v>
@@ -2432,7 +2423,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>8</v>
@@ -2443,7 +2434,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>5</v>
@@ -2457,7 +2448,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>5</v>
@@ -2471,7 +2462,7 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>8</v>
@@ -2482,7 +2473,7 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>5</v>
@@ -2496,7 +2487,7 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>5</v>
@@ -2510,7 +2501,7 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>8</v>
@@ -2521,7 +2512,7 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>5</v>
@@ -2535,7 +2526,7 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>5</v>
@@ -2549,7 +2540,7 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>8</v>
@@ -2560,7 +2551,7 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>5</v>
@@ -2574,7 +2565,7 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>5</v>
@@ -2588,7 +2579,7 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>8</v>
@@ -2599,7 +2590,7 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>5</v>
@@ -2613,7 +2604,7 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>5</v>
@@ -2627,7 +2618,7 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>8</v>
@@ -2638,7 +2629,7 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>5</v>
@@ -2652,7 +2643,7 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>5</v>
@@ -2666,7 +2657,7 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>8</v>
@@ -2677,13 +2668,13 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>45</v>
-      </c>
-      <c r="B50" s="6" t="s">
-        <v>60</v>
+        <v>40</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>55</v>
       </c>
       <c r="C50" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="D50" t="s">
         <v>13</v>
@@ -2691,9 +2682,9 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>45</v>
-      </c>
-      <c r="B51" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B51" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C51" t="s">
@@ -2705,80 +2696,80 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>45</v>
-      </c>
-      <c r="B52" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B52" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C52" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="D52" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>45</v>
-      </c>
-      <c r="B53" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B53" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D53" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>54</v>
-      </c>
-      <c r="B54" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C54" t="s">
+        <v>58</v>
+      </c>
+      <c r="D54" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B55" s="7">
+        <v>2</v>
+      </c>
+      <c r="C55" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D55" s="6" t="s">
         <v>60</v>
-      </c>
-      <c r="C54" t="s">
-        <v>63</v>
-      </c>
-      <c r="D54" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A55" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="B55" s="8">
-        <v>2</v>
-      </c>
-      <c r="C55" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="D55" s="7" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>54</v>
-      </c>
-      <c r="B56" s="6" t="s">
-        <v>60</v>
+        <v>49</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>55</v>
       </c>
       <c r="C56" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="D56" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>54</v>
-      </c>
-      <c r="B57" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B57" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D57" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated PTEN in consolidation sheet
</commit_message>
<xml_diff>
--- a/inst/extdata/biomarker_rules_enoc.xlsx
+++ b/inst/extdata/biomarker_rules_enoc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hannahokada/Documents/GitHub/EDGEResearch - CA:TMATools/TMAtools/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0F21FEA-5D8A-AE4E-AF36-FF183BFCFE54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27A4AE31-2BD3-8149-AA0C-EB6094648FDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16340" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="65">
   <si>
     <t>biomarker</t>
   </si>
@@ -99,9 +99,6 @@
   </si>
   <si>
     <t>retained</t>
-  </si>
-  <si>
-    <t>all</t>
   </si>
   <si>
     <t>equivocal blush</t>
@@ -259,18 +256,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -292,7 +283,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -307,9 +298,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="3" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -635,10 +624,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -690,7 +679,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
@@ -709,7 +698,7 @@
     </row>
     <row r="8" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B8" s="4">
         <v>0</v>
@@ -720,7 +709,7 @@
     </row>
     <row r="9" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B9" s="4">
         <v>1</v>
@@ -731,7 +720,7 @@
     </row>
     <row r="10" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B10" s="4">
         <v>2</v>
@@ -742,7 +731,7 @@
     </row>
     <row r="11" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B11" s="4">
         <v>3</v>
@@ -753,7 +742,7 @@
     </row>
     <row r="12" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B12" s="4">
         <v>4</v>
@@ -764,7 +753,7 @@
     </row>
     <row r="13" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B13" s="4">
         <v>5</v>
@@ -775,7 +764,7 @@
     </row>
     <row r="14" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B14" s="4">
         <v>8</v>
@@ -786,7 +775,7 @@
     </row>
     <row r="15" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B15" s="4">
         <v>9</v>
@@ -797,10 +786,10 @@
     </row>
     <row r="16" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C16" t="s">
         <v>11</v>
@@ -808,7 +797,7 @@
     </row>
     <row r="17" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>11</v>
@@ -888,10 +877,10 @@
         <v>19</v>
       </c>
       <c r="B24" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C24" t="s">
         <v>32</v>
-      </c>
-      <c r="C24" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -899,7 +888,7 @@
         <v>19</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C25" t="s">
         <v>11</v>
@@ -924,7 +913,7 @@
         <v>1</v>
       </c>
       <c r="C27" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -935,7 +924,7 @@
         <v>2</v>
       </c>
       <c r="C28" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -968,7 +957,7 @@
         <v>5</v>
       </c>
       <c r="C31" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -987,7 +976,7 @@
         <v>23</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C33" t="s">
         <v>11</v>
@@ -1006,7 +995,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B35" s="4">
         <v>0</v>
@@ -1017,7 +1006,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B36" s="4">
         <v>1</v>
@@ -1028,7 +1017,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B37" s="4">
         <v>2</v>
@@ -1039,7 +1028,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B38" s="4">
         <v>9</v>
@@ -1050,10 +1039,10 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C39" t="s">
         <v>11</v>
@@ -1061,7 +1050,7 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>11</v>
@@ -1072,7 +1061,7 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B41" s="4">
         <v>0</v>
@@ -1083,7 +1072,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B42" s="4">
         <v>1</v>
@@ -1094,7 +1083,7 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B43" s="4">
         <v>2</v>
@@ -1105,7 +1094,7 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B44" s="4">
         <v>9</v>
@@ -1116,10 +1105,10 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C45" t="s">
         <v>11</v>
@@ -1127,7 +1116,7 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>11</v>
@@ -1138,7 +1127,7 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B47" s="4">
         <v>0</v>
@@ -1149,7 +1138,7 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B48" s="4">
         <v>1</v>
@@ -1160,7 +1149,7 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B49" s="4">
         <v>2</v>
@@ -1171,7 +1160,7 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B50" s="4">
         <v>9</v>
@@ -1182,10 +1171,10 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C51" t="s">
         <v>11</v>
@@ -1193,7 +1182,7 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B52" s="3" t="s">
         <v>11</v>
@@ -1204,7 +1193,7 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B53" s="4">
         <v>0</v>
@@ -1215,7 +1204,7 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B54" s="4">
         <v>1</v>
@@ -1226,7 +1215,7 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B55" s="4">
         <v>2</v>
@@ -1237,7 +1226,7 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B56" s="4">
         <v>9</v>
@@ -1248,10 +1237,10 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C57" t="s">
         <v>11</v>
@@ -1259,7 +1248,7 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B58" s="3" t="s">
         <v>11</v>
@@ -1270,7 +1259,7 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B59" s="4">
         <v>0</v>
@@ -1281,7 +1270,7 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B60" s="4">
         <v>1</v>
@@ -1292,7 +1281,7 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B61" s="4">
         <v>2</v>
@@ -1303,7 +1292,7 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B62" s="4">
         <v>9</v>
@@ -1314,10 +1303,10 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C63" t="s">
         <v>11</v>
@@ -1325,7 +1314,7 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B64" s="3" t="s">
         <v>11</v>
@@ -1336,7 +1325,7 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B65" s="4">
         <v>0</v>
@@ -1347,7 +1336,7 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B66" s="4">
         <v>1</v>
@@ -1358,7 +1347,7 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B67" s="4">
         <v>2</v>
@@ -1369,7 +1358,7 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B68" s="4">
         <v>9</v>
@@ -1380,10 +1369,10 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C69" t="s">
         <v>11</v>
@@ -1391,7 +1380,7 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B70" s="3" t="s">
         <v>11</v>
@@ -1402,7 +1391,7 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B71" s="5">
         <v>0</v>
@@ -1413,54 +1402,54 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B72" s="5">
         <v>1</v>
       </c>
       <c r="C72" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B73" s="5">
         <v>2</v>
       </c>
       <c r="C73" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B74" s="5">
         <v>3</v>
       </c>
       <c r="C74" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B75" s="5">
         <v>9</v>
       </c>
       <c r="C75" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B76" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C76" t="s">
         <v>11</v>
@@ -1468,7 +1457,7 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B77" s="5" t="s">
         <v>11</v>
@@ -1479,7 +1468,7 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B78" s="4">
         <v>0</v>
@@ -1490,7 +1479,7 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B79" s="4">
         <v>1</v>
@@ -1501,7 +1490,7 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B80" s="4">
         <v>2</v>
@@ -1512,7 +1501,7 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B81" s="4">
         <v>3</v>
@@ -1523,7 +1512,7 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B82" s="4">
         <v>8</v>
@@ -1534,7 +1523,7 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B83" s="4">
         <v>9</v>
@@ -1545,10 +1534,10 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C84" t="s">
         <v>11</v>
@@ -1556,18 +1545,18 @@
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C85" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B86" s="4">
         <v>0</v>
@@ -1578,7 +1567,7 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B87" s="4">
         <v>1</v>
@@ -1589,7 +1578,7 @@
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B88" s="4">
         <v>2</v>
@@ -1600,7 +1589,7 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B89" s="4">
         <v>3</v>
@@ -1611,7 +1600,7 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B90" s="4">
         <v>8</v>
@@ -1622,7 +1611,7 @@
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B91" s="4">
         <v>9</v>
@@ -1633,10 +1622,10 @@
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C92" t="s">
         <v>11</v>
@@ -1644,18 +1633,18 @@
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C93" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B94" s="4">
         <v>0</v>
@@ -1666,7 +1655,7 @@
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B95" s="4">
         <v>1</v>
@@ -1677,7 +1666,7 @@
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B96" s="4">
         <v>2</v>
@@ -1688,7 +1677,7 @@
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B97" s="4">
         <v>3</v>
@@ -1699,7 +1688,7 @@
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B98" s="4">
         <v>8</v>
@@ -1710,7 +1699,7 @@
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B99" s="4">
         <v>9</v>
@@ -1721,21 +1710,21 @@
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B100" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C100" t="s">
         <v>32</v>
-      </c>
-      <c r="C100" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B101" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C101" t="s">
         <v>11</v>
@@ -1743,7 +1732,7 @@
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B102" s="4">
         <v>0</v>
@@ -1754,7 +1743,7 @@
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B103" s="4">
         <v>1</v>
@@ -1765,7 +1754,7 @@
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B104" s="4">
         <v>2</v>
@@ -1776,7 +1765,7 @@
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B105" s="4">
         <v>3</v>
@@ -1787,7 +1776,7 @@
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B106" s="4">
         <v>8</v>
@@ -1798,7 +1787,7 @@
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B107" s="4">
         <v>9</v>
@@ -1809,10 +1798,10 @@
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C108" t="s">
         <v>11</v>
@@ -1820,10 +1809,10 @@
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C109" t="s">
         <v>11</v>
@@ -1831,7 +1820,7 @@
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B110" s="4">
         <v>0</v>
@@ -1842,7 +1831,7 @@
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B111" s="4">
         <v>1</v>
@@ -1853,7 +1842,7 @@
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B112" s="4">
         <v>2</v>
@@ -1864,7 +1853,7 @@
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B113" s="4">
         <v>3</v>
@@ -1875,7 +1864,7 @@
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B114" s="4">
         <v>8</v>
@@ -1886,7 +1875,7 @@
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B115" s="4">
         <v>9</v>
@@ -1897,10 +1886,10 @@
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C116" t="s">
         <v>11</v>
@@ -1908,90 +1897,90 @@
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C117" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B118" s="5">
         <v>0</v>
       </c>
       <c r="C118" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B119" s="5">
         <v>1</v>
       </c>
       <c r="C119" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B120" s="5">
         <v>2</v>
       </c>
       <c r="C120" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B121" s="5">
         <v>3</v>
       </c>
       <c r="C121" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B122" s="5">
         <v>9</v>
       </c>
       <c r="C122" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B123" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C123" t="s">
         <v>32</v>
-      </c>
-      <c r="C123" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B124" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C124" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -2007,8 +1996,8 @@
   </sheetPr>
   <dimension ref="A1:D57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="220" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" zoomScale="111" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2197,10 +2186,10 @@
         <v>23</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D14" t="s">
         <v>17</v>
@@ -2210,11 +2199,11 @@
       <c r="A15" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="8">
-        <v>2</v>
+      <c r="B15" s="6" t="s">
+        <v>24</v>
       </c>
       <c r="C15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D15" t="s">
         <v>17</v>
@@ -2224,11 +2213,11 @@
       <c r="A16" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="6" t="s">
         <v>24</v>
       </c>
       <c r="C16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D16" t="s">
         <v>17</v>
@@ -2238,8 +2227,8 @@
       <c r="A17" t="s">
         <v>23</v>
       </c>
-      <c r="B17" s="8" t="s">
-        <v>26</v>
+      <c r="B17" s="6" t="s">
+        <v>54</v>
       </c>
       <c r="C17" t="s">
         <v>20</v>
@@ -2252,7 +2241,7 @@
       <c r="A18" t="s">
         <v>23</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C18" t="s">
@@ -2266,11 +2255,11 @@
       <c r="A19" t="s">
         <v>23</v>
       </c>
-      <c r="B19" s="8" t="s">
-        <v>55</v>
+      <c r="B19" s="6" t="s">
+        <v>54</v>
       </c>
       <c r="C19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D19" t="s">
         <v>11</v>
@@ -2280,11 +2269,11 @@
       <c r="A20" t="s">
         <v>23</v>
       </c>
-      <c r="B20" s="8" t="s">
-        <v>55</v>
+      <c r="B20" s="6" t="s">
+        <v>54</v>
       </c>
       <c r="C20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D20" t="s">
         <v>11</v>
@@ -2294,14 +2283,14 @@
       <c r="A21" t="s">
         <v>23</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="B21" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -2312,12 +2301,12 @@
         <v>8</v>
       </c>
       <c r="D22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>5</v>
@@ -2331,7 +2320,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>5</v>
@@ -2345,7 +2334,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>8</v>
@@ -2356,7 +2345,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>5</v>
@@ -2370,7 +2359,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>5</v>
@@ -2384,7 +2373,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>8</v>
@@ -2395,7 +2384,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>5</v>
@@ -2409,7 +2398,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>5</v>
@@ -2423,7 +2412,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>8</v>
@@ -2434,7 +2423,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>5</v>
@@ -2448,7 +2437,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>5</v>
@@ -2462,7 +2451,7 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>8</v>
@@ -2473,7 +2462,7 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>5</v>
@@ -2487,7 +2476,7 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>5</v>
@@ -2501,7 +2490,7 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>8</v>
@@ -2512,7 +2501,7 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>5</v>
@@ -2526,7 +2515,7 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>5</v>
@@ -2540,7 +2529,7 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>8</v>
@@ -2551,7 +2540,7 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>5</v>
@@ -2565,7 +2554,7 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>5</v>
@@ -2579,7 +2568,7 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>8</v>
@@ -2590,7 +2579,7 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>5</v>
@@ -2604,7 +2593,7 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>5</v>
@@ -2618,7 +2607,7 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>8</v>
@@ -2629,7 +2618,7 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>5</v>
@@ -2643,7 +2632,7 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>5</v>
@@ -2657,7 +2646,7 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>8</v>
@@ -2668,13 +2657,13 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B50" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C50" t="s">
         <v>55</v>
-      </c>
-      <c r="C50" t="s">
-        <v>56</v>
       </c>
       <c r="D50" t="s">
         <v>13</v>
@@ -2682,7 +2671,7 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B51" s="5" t="s">
         <v>5</v>
@@ -2696,80 +2685,80 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
+        <v>39</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C52" t="s">
         <v>40</v>
       </c>
-      <c r="B52" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C52" t="s">
-        <v>41</v>
-      </c>
       <c r="D52" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B53" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D53" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C54" t="s">
+        <v>57</v>
+      </c>
+      <c r="D54" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>48</v>
+      </c>
+      <c r="B55" s="5">
+        <v>2</v>
+      </c>
+      <c r="C55" t="s">
         <v>58</v>
       </c>
-      <c r="D54" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A55" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="B55" s="7">
-        <v>2</v>
-      </c>
-      <c r="C55" s="6" t="s">
+      <c r="D55" t="s">
         <v>59</v>
-      </c>
-      <c r="D55" s="6" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C56" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D56" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B57" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D57" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Edited p16 in consolidation sheet
</commit_message>
<xml_diff>
--- a/inst/extdata/biomarker_rules_enoc.xlsx
+++ b/inst/extdata/biomarker_rules_enoc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hannahokada/Documents/GitHub/EDGEResearch - CA:TMATools/TMAtools/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C66AAEC-528E-3B4A-91E3-42CB1D057879}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BADC3041-B548-7543-86C4-7FD9269E8729}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16340" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="65">
   <si>
     <t>biomarker</t>
   </si>
@@ -197,9 +197,6 @@
     <t xml:space="preserve">normal </t>
   </si>
   <si>
-    <t xml:space="preserve">Abnormal complete absence &amp; abnormal block </t>
-  </si>
-  <si>
     <t xml:space="preserve">duo abnormal </t>
   </si>
   <si>
@@ -216,6 +213,9 @@
   </si>
   <si>
     <t>absent;reduced</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Abnormal complete absence;abnormal block </t>
   </si>
 </sst>
 </file>
@@ -695,7 +695,7 @@
     </row>
     <row r="8" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B8" s="4">
         <v>0</v>
@@ -706,7 +706,7 @@
     </row>
     <row r="9" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B9" s="4">
         <v>1</v>
@@ -717,7 +717,7 @@
     </row>
     <row r="10" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B10" s="4">
         <v>2</v>
@@ -728,7 +728,7 @@
     </row>
     <row r="11" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B11" s="4">
         <v>3</v>
@@ -739,7 +739,7 @@
     </row>
     <row r="12" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B12" s="4">
         <v>4</v>
@@ -750,7 +750,7 @@
     </row>
     <row r="13" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B13" s="4">
         <v>5</v>
@@ -761,7 +761,7 @@
     </row>
     <row r="14" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B14" s="4">
         <v>8</v>
@@ -772,7 +772,7 @@
     </row>
     <row r="15" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B15" s="4">
         <v>9</v>
@@ -783,7 +783,7 @@
     </row>
     <row r="16" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>31</v>
@@ -794,7 +794,7 @@
     </row>
     <row r="17" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>11</v>
@@ -1993,8 +1993,8 @@
   </sheetPr>
   <dimension ref="A1:D57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="111" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" zoomScale="111" workbookViewId="0">
+      <selection activeCell="G52" sqref="G52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2186,7 +2186,7 @@
         <v>54</v>
       </c>
       <c r="C14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D14" t="s">
         <v>17</v>
@@ -2200,7 +2200,7 @@
         <v>24</v>
       </c>
       <c r="C15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D15" t="s">
         <v>17</v>
@@ -2214,7 +2214,7 @@
         <v>24</v>
       </c>
       <c r="C16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D16" t="s">
         <v>17</v>
@@ -2723,14 +2723,14 @@
       <c r="A55" t="s">
         <v>48</v>
       </c>
-      <c r="B55" s="5">
-        <v>2</v>
+      <c r="B55" s="5" t="s">
+        <v>24</v>
       </c>
       <c r="C55" t="s">
+        <v>64</v>
+      </c>
+      <c r="D55" t="s">
         <v>58</v>
-      </c>
-      <c r="D55" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
@@ -2755,7 +2755,7 @@
         <v>8</v>
       </c>
       <c r="D57" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
documenting consolidate_single_patient function, and updating docs
</commit_message>
<xml_diff>
--- a/inst/extdata/biomarker_rules_enoc.xlsx
+++ b/inst/extdata/biomarker_rules_enoc.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hannahokada/Documents/GitHub/EDGEResearch - CA:TMATools/TMAtools/inst/extdata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ubcca-my.sharepoint.com/personal/bianca_ribeiro_ubc_ca/Documents/TMAtools/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C66AAEC-528E-3B4A-91E3-42CB1D057879}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{9C66AAEC-528E-3B4A-91E3-42CB1D057879}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{298E836D-5175-40D9-B6A2-3D0622A48D1E}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16340" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14130" yWindow="2340" windowWidth="14805" windowHeight="13095" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="translation" sheetId="1" r:id="rId1"/>
@@ -609,14 +609,14 @@
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.83203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -627,7 +627,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -638,7 +638,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -649,7 +649,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -660,7 +660,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -671,7 +671,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -682,7 +682,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -693,7 +693,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>62</v>
       </c>
@@ -704,7 +704,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>62</v>
       </c>
@@ -715,7 +715,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>62</v>
       </c>
@@ -726,7 +726,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>62</v>
       </c>
@@ -737,7 +737,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>62</v>
       </c>
@@ -748,7 +748,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>62</v>
       </c>
@@ -759,7 +759,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>62</v>
       </c>
@@ -770,7 +770,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>62</v>
       </c>
@@ -781,7 +781,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>62</v>
       </c>
@@ -792,7 +792,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>62</v>
       </c>
@@ -803,7 +803,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -814,7 +814,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -825,7 +825,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -836,7 +836,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -847,7 +847,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>19</v>
       </c>
@@ -858,7 +858,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>19</v>
       </c>
@@ -869,7 +869,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>19</v>
       </c>
@@ -880,7 +880,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>19</v>
       </c>
@@ -891,7 +891,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>23</v>
       </c>
@@ -902,7 +902,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>23</v>
       </c>
@@ -913,7 +913,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>23</v>
       </c>
@@ -924,7 +924,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>23</v>
       </c>
@@ -935,7 +935,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>23</v>
       </c>
@@ -946,7 +946,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>23</v>
       </c>
@@ -957,7 +957,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>23</v>
       </c>
@@ -968,7 +968,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>23</v>
       </c>
@@ -979,7 +979,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>23</v>
       </c>
@@ -990,7 +990,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>33</v>
       </c>
@@ -1001,7 +1001,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>33</v>
       </c>
@@ -1012,7 +1012,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>33</v>
       </c>
@@ -1023,7 +1023,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>33</v>
       </c>
@@ -1034,7 +1034,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>33</v>
       </c>
@@ -1045,7 +1045,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>33</v>
       </c>
@@ -1056,7 +1056,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>34</v>
       </c>
@@ -1067,7 +1067,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>34</v>
       </c>
@@ -1078,7 +1078,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>34</v>
       </c>
@@ -1089,7 +1089,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>34</v>
       </c>
@@ -1100,7 +1100,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>34</v>
       </c>
@@ -1111,7 +1111,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>34</v>
       </c>
@@ -1122,7 +1122,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>35</v>
       </c>
@@ -1133,7 +1133,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>35</v>
       </c>
@@ -1144,7 +1144,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>35</v>
       </c>
@@ -1155,7 +1155,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>35</v>
       </c>
@@ -1166,7 +1166,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>35</v>
       </c>
@@ -1177,7 +1177,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>35</v>
       </c>
@@ -1188,7 +1188,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>36</v>
       </c>
@@ -1199,7 +1199,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>36</v>
       </c>
@@ -1210,7 +1210,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>36</v>
       </c>
@@ -1221,7 +1221,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>36</v>
       </c>
@@ -1232,7 +1232,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>36</v>
       </c>
@@ -1243,7 +1243,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>36</v>
       </c>
@@ -1254,7 +1254,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>37</v>
       </c>
@@ -1265,7 +1265,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>37</v>
       </c>
@@ -1276,7 +1276,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>37</v>
       </c>
@@ -1287,7 +1287,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>37</v>
       </c>
@@ -1298,7 +1298,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>37</v>
       </c>
@@ -1309,7 +1309,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>37</v>
       </c>
@@ -1320,7 +1320,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>38</v>
       </c>
@@ -1331,7 +1331,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>38</v>
       </c>
@@ -1342,7 +1342,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>38</v>
       </c>
@@ -1353,7 +1353,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>38</v>
       </c>
@@ -1364,7 +1364,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>38</v>
       </c>
@@ -1375,7 +1375,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>38</v>
       </c>
@@ -1386,7 +1386,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>39</v>
       </c>
@@ -1397,7 +1397,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>39</v>
       </c>
@@ -1408,7 +1408,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>39</v>
       </c>
@@ -1419,7 +1419,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>39</v>
       </c>
@@ -1430,7 +1430,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>39</v>
       </c>
@@ -1441,7 +1441,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>39</v>
       </c>
@@ -1452,7 +1452,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>39</v>
       </c>
@@ -1463,7 +1463,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>42</v>
       </c>
@@ -1474,7 +1474,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>42</v>
       </c>
@@ -1485,7 +1485,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>42</v>
       </c>
@@ -1496,7 +1496,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>42</v>
       </c>
@@ -1507,7 +1507,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>42</v>
       </c>
@@ -1518,7 +1518,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>42</v>
       </c>
@@ -1529,7 +1529,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>42</v>
       </c>
@@ -1540,7 +1540,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>42</v>
       </c>
@@ -1551,7 +1551,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>43</v>
       </c>
@@ -1562,7 +1562,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>43</v>
       </c>
@@ -1573,7 +1573,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>43</v>
       </c>
@@ -1584,7 +1584,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>44</v>
       </c>
@@ -1595,7 +1595,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>44</v>
       </c>
@@ -1606,7 +1606,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>44</v>
       </c>
@@ -1617,7 +1617,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>44</v>
       </c>
@@ -1628,7 +1628,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>43</v>
       </c>
@@ -1639,7 +1639,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>45</v>
       </c>
@@ -1650,7 +1650,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>45</v>
       </c>
@@ -1661,7 +1661,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>45</v>
       </c>
@@ -1672,7 +1672,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>45</v>
       </c>
@@ -1683,7 +1683,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>45</v>
       </c>
@@ -1694,7 +1694,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>45</v>
       </c>
@@ -1705,7 +1705,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>45</v>
       </c>
@@ -1716,7 +1716,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>45</v>
       </c>
@@ -1727,7 +1727,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>46</v>
       </c>
@@ -1738,7 +1738,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>46</v>
       </c>
@@ -1749,7 +1749,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>46</v>
       </c>
@@ -1760,7 +1760,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>46</v>
       </c>
@@ -1771,7 +1771,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>46</v>
       </c>
@@ -1782,7 +1782,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>46</v>
       </c>
@@ -1793,7 +1793,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>46</v>
       </c>
@@ -1804,7 +1804,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>46</v>
       </c>
@@ -1815,7 +1815,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>47</v>
       </c>
@@ -1826,7 +1826,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>47</v>
       </c>
@@ -1837,7 +1837,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>47</v>
       </c>
@@ -1848,7 +1848,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>47</v>
       </c>
@@ -1859,7 +1859,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>47</v>
       </c>
@@ -1870,7 +1870,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>47</v>
       </c>
@@ -1881,7 +1881,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>47</v>
       </c>
@@ -1892,7 +1892,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>47</v>
       </c>
@@ -1903,7 +1903,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>48</v>
       </c>
@@ -1914,7 +1914,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>48</v>
       </c>
@@ -1925,7 +1925,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>48</v>
       </c>
@@ -1936,7 +1936,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>52</v>
       </c>
@@ -1947,7 +1947,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>52</v>
       </c>
@@ -1958,7 +1958,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>52</v>
       </c>
@@ -1969,7 +1969,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>48</v>
       </c>
@@ -1993,19 +1993,19 @@
   </sheetPr>
   <dimension ref="A1:D57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="111" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="111" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2019,7 +2019,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -2033,7 +2033,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -2047,7 +2047,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -2058,7 +2058,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -2072,7 +2072,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -2086,7 +2086,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -2100,7 +2100,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -2114,7 +2114,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -2128,7 +2128,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -2139,7 +2139,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -2153,7 +2153,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -2167,7 +2167,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -2178,7 +2178,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>23</v>
       </c>
@@ -2192,7 +2192,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -2206,7 +2206,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -2220,7 +2220,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -2234,7 +2234,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>23</v>
       </c>
@@ -2248,7 +2248,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>23</v>
       </c>
@@ -2262,7 +2262,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -2276,7 +2276,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>23</v>
       </c>
@@ -2290,7 +2290,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -2301,7 +2301,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>33</v>
       </c>
@@ -2315,7 +2315,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>33</v>
       </c>
@@ -2329,7 +2329,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>53</v>
       </c>
@@ -2340,7 +2340,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>35</v>
       </c>
@@ -2354,7 +2354,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>35</v>
       </c>
@@ -2368,7 +2368,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>35</v>
       </c>
@@ -2379,7 +2379,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>36</v>
       </c>
@@ -2393,7 +2393,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>36</v>
       </c>
@@ -2407,7 +2407,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>36</v>
       </c>
@@ -2418,7 +2418,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>37</v>
       </c>
@@ -2432,7 +2432,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>37</v>
       </c>
@@ -2446,7 +2446,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>37</v>
       </c>
@@ -2457,7 +2457,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>38</v>
       </c>
@@ -2471,7 +2471,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>38</v>
       </c>
@@ -2485,7 +2485,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>38</v>
       </c>
@@ -2496,7 +2496,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>42</v>
       </c>
@@ -2510,7 +2510,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>42</v>
       </c>
@@ -2524,7 +2524,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>42</v>
       </c>
@@ -2535,7 +2535,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>45</v>
       </c>
@@ -2549,7 +2549,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>45</v>
       </c>
@@ -2563,7 +2563,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>45</v>
       </c>
@@ -2574,7 +2574,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>46</v>
       </c>
@@ -2588,7 +2588,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>46</v>
       </c>
@@ -2602,7 +2602,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>46</v>
       </c>
@@ -2613,7 +2613,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>47</v>
       </c>
@@ -2627,7 +2627,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>47</v>
       </c>
@@ -2641,7 +2641,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>47</v>
       </c>
@@ -2652,7 +2652,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>39</v>
       </c>
@@ -2666,7 +2666,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>39</v>
       </c>
@@ -2680,7 +2680,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>39</v>
       </c>
@@ -2694,7 +2694,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>39</v>
       </c>
@@ -2705,7 +2705,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>48</v>
       </c>
@@ -2719,7 +2719,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>48</v>
       </c>
@@ -2733,7 +2733,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>48</v>
       </c>
@@ -2747,7 +2747,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>48</v>
       </c>

</xml_diff>

<commit_message>
Fixed error in combined_tma_sheets
</commit_message>
<xml_diff>
--- a/inst/extdata/biomarker_rules_enoc.xlsx
+++ b/inst/extdata/biomarker_rules_enoc.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11018"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ubcca-my.sharepoint.com/personal/bianca_ribeiro_ubc_ca/Documents/TMAtools/inst/extdata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hannahokada/Documents/TMAtools/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{9C66AAEC-528E-3B4A-91E3-42CB1D057879}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{298E836D-5175-40D9-B6A2-3D0622A48D1E}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4DB5EE6-EEA5-1644-BC70-4061F8FFD127}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14130" yWindow="2340" windowWidth="14805" windowHeight="13095" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14000" yWindow="2340" windowWidth="14800" windowHeight="13100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="translation" sheetId="1" r:id="rId1"/>
@@ -609,14 +609,14 @@
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.83203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -627,7 +627,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -638,7 +638,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -649,7 +649,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -660,7 +660,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -671,7 +671,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -682,7 +682,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -693,7 +693,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>62</v>
       </c>
@@ -704,7 +704,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>62</v>
       </c>
@@ -715,7 +715,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>62</v>
       </c>
@@ -726,7 +726,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>62</v>
       </c>
@@ -737,7 +737,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>62</v>
       </c>
@@ -748,7 +748,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>62</v>
       </c>
@@ -759,7 +759,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>62</v>
       </c>
@@ -770,7 +770,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>62</v>
       </c>
@@ -781,7 +781,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>62</v>
       </c>
@@ -792,7 +792,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>62</v>
       </c>
@@ -803,7 +803,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -814,7 +814,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -825,7 +825,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -836,7 +836,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -847,7 +847,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>19</v>
       </c>
@@ -858,7 +858,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>19</v>
       </c>
@@ -869,7 +869,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>19</v>
       </c>
@@ -880,7 +880,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>19</v>
       </c>
@@ -891,7 +891,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>23</v>
       </c>
@@ -902,7 +902,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>23</v>
       </c>
@@ -913,7 +913,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>23</v>
       </c>
@@ -924,7 +924,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>23</v>
       </c>
@@ -935,7 +935,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>23</v>
       </c>
@@ -946,7 +946,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>23</v>
       </c>
@@ -957,7 +957,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>23</v>
       </c>
@@ -968,7 +968,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>23</v>
       </c>
@@ -979,7 +979,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>23</v>
       </c>
@@ -990,7 +990,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>33</v>
       </c>
@@ -1001,7 +1001,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>33</v>
       </c>
@@ -1012,7 +1012,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>33</v>
       </c>
@@ -1023,7 +1023,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>33</v>
       </c>
@@ -1034,7 +1034,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>33</v>
       </c>
@@ -1045,7 +1045,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>33</v>
       </c>
@@ -1056,7 +1056,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>34</v>
       </c>
@@ -1067,7 +1067,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>34</v>
       </c>
@@ -1078,7 +1078,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>34</v>
       </c>
@@ -1089,7 +1089,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>34</v>
       </c>
@@ -1100,7 +1100,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>34</v>
       </c>
@@ -1111,7 +1111,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>34</v>
       </c>
@@ -1122,7 +1122,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>35</v>
       </c>
@@ -1133,7 +1133,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>35</v>
       </c>
@@ -1144,7 +1144,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>35</v>
       </c>
@@ -1155,7 +1155,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>35</v>
       </c>
@@ -1166,7 +1166,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>35</v>
       </c>
@@ -1177,7 +1177,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>35</v>
       </c>
@@ -1188,7 +1188,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>36</v>
       </c>
@@ -1199,7 +1199,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>36</v>
       </c>
@@ -1210,7 +1210,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>36</v>
       </c>
@@ -1221,7 +1221,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>36</v>
       </c>
@@ -1232,7 +1232,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>36</v>
       </c>
@@ -1243,7 +1243,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>36</v>
       </c>
@@ -1254,7 +1254,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>37</v>
       </c>
@@ -1265,7 +1265,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>37</v>
       </c>
@@ -1276,7 +1276,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>37</v>
       </c>
@@ -1287,7 +1287,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>37</v>
       </c>
@@ -1298,7 +1298,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>37</v>
       </c>
@@ -1309,7 +1309,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>37</v>
       </c>
@@ -1320,7 +1320,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>38</v>
       </c>
@@ -1331,7 +1331,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>38</v>
       </c>
@@ -1342,7 +1342,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>38</v>
       </c>
@@ -1353,7 +1353,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>38</v>
       </c>
@@ -1364,7 +1364,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>38</v>
       </c>
@@ -1375,7 +1375,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>38</v>
       </c>
@@ -1386,7 +1386,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>39</v>
       </c>
@@ -1397,7 +1397,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>39</v>
       </c>
@@ -1408,7 +1408,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>39</v>
       </c>
@@ -1419,7 +1419,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>39</v>
       </c>
@@ -1430,7 +1430,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>39</v>
       </c>
@@ -1441,7 +1441,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>39</v>
       </c>
@@ -1452,7 +1452,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>39</v>
       </c>
@@ -1463,7 +1463,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>42</v>
       </c>
@@ -1474,7 +1474,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>42</v>
       </c>
@@ -1485,7 +1485,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>42</v>
       </c>
@@ -1496,7 +1496,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>42</v>
       </c>
@@ -1507,7 +1507,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>42</v>
       </c>
@@ -1518,7 +1518,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>42</v>
       </c>
@@ -1529,7 +1529,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>42</v>
       </c>
@@ -1540,7 +1540,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>42</v>
       </c>
@@ -1551,7 +1551,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>43</v>
       </c>
@@ -1562,7 +1562,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>43</v>
       </c>
@@ -1573,7 +1573,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>43</v>
       </c>
@@ -1584,7 +1584,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>44</v>
       </c>
@@ -1595,7 +1595,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>44</v>
       </c>
@@ -1606,7 +1606,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>44</v>
       </c>
@@ -1617,7 +1617,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>44</v>
       </c>
@@ -1628,7 +1628,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>43</v>
       </c>
@@ -1639,7 +1639,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>45</v>
       </c>
@@ -1650,7 +1650,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>45</v>
       </c>
@@ -1661,7 +1661,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>45</v>
       </c>
@@ -1672,7 +1672,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>45</v>
       </c>
@@ -1683,7 +1683,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>45</v>
       </c>
@@ -1694,7 +1694,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>45</v>
       </c>
@@ -1705,7 +1705,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>45</v>
       </c>
@@ -1716,7 +1716,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>45</v>
       </c>
@@ -1727,7 +1727,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>46</v>
       </c>
@@ -1738,7 +1738,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>46</v>
       </c>
@@ -1749,7 +1749,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>46</v>
       </c>
@@ -1760,7 +1760,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>46</v>
       </c>
@@ -1771,7 +1771,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>46</v>
       </c>
@@ -1782,7 +1782,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>46</v>
       </c>
@@ -1793,7 +1793,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>46</v>
       </c>
@@ -1804,7 +1804,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>46</v>
       </c>
@@ -1815,7 +1815,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>47</v>
       </c>
@@ -1826,7 +1826,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>47</v>
       </c>
@@ -1837,7 +1837,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>47</v>
       </c>
@@ -1848,7 +1848,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>47</v>
       </c>
@@ -1859,7 +1859,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>47</v>
       </c>
@@ -1870,7 +1870,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>47</v>
       </c>
@@ -1881,7 +1881,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>47</v>
       </c>
@@ -1892,7 +1892,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>47</v>
       </c>
@@ -1903,7 +1903,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>48</v>
       </c>
@@ -1914,7 +1914,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>48</v>
       </c>
@@ -1925,7 +1925,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>48</v>
       </c>
@@ -1936,7 +1936,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>52</v>
       </c>
@@ -1947,7 +1947,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>52</v>
       </c>
@@ -1958,7 +1958,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>52</v>
       </c>
@@ -1969,7 +1969,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>48</v>
       </c>
@@ -1993,19 +1993,19 @@
   </sheetPr>
   <dimension ref="A1:D57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="111" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="111" workbookViewId="0">
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2019,7 +2019,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -2033,7 +2033,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -2047,7 +2047,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -2058,7 +2058,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -2072,7 +2072,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -2086,7 +2086,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -2100,7 +2100,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -2114,7 +2114,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -2128,7 +2128,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -2139,7 +2139,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -2153,7 +2153,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -2167,7 +2167,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -2178,7 +2178,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>23</v>
       </c>
@@ -2192,7 +2192,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -2206,7 +2206,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -2220,7 +2220,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -2234,7 +2234,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>23</v>
       </c>
@@ -2248,7 +2248,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>23</v>
       </c>
@@ -2262,7 +2262,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -2276,7 +2276,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>23</v>
       </c>
@@ -2290,7 +2290,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -2301,7 +2301,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>33</v>
       </c>
@@ -2315,7 +2315,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>33</v>
       </c>
@@ -2329,7 +2329,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>53</v>
       </c>
@@ -2340,7 +2340,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>35</v>
       </c>
@@ -2354,7 +2354,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>35</v>
       </c>
@@ -2368,7 +2368,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>35</v>
       </c>
@@ -2379,7 +2379,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>36</v>
       </c>
@@ -2393,7 +2393,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>36</v>
       </c>
@@ -2407,7 +2407,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>36</v>
       </c>
@@ -2418,7 +2418,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>37</v>
       </c>
@@ -2432,7 +2432,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>37</v>
       </c>
@@ -2446,7 +2446,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>37</v>
       </c>
@@ -2457,7 +2457,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>38</v>
       </c>
@@ -2471,7 +2471,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>38</v>
       </c>
@@ -2485,7 +2485,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>38</v>
       </c>
@@ -2496,7 +2496,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>42</v>
       </c>
@@ -2510,7 +2510,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>42</v>
       </c>
@@ -2524,7 +2524,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>42</v>
       </c>
@@ -2535,7 +2535,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>45</v>
       </c>
@@ -2549,7 +2549,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>45</v>
       </c>
@@ -2563,7 +2563,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>45</v>
       </c>
@@ -2574,7 +2574,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>46</v>
       </c>
@@ -2588,7 +2588,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>46</v>
       </c>
@@ -2602,7 +2602,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>46</v>
       </c>
@@ -2613,7 +2613,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>47</v>
       </c>
@@ -2627,7 +2627,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>47</v>
       </c>
@@ -2641,7 +2641,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>47</v>
       </c>
@@ -2652,7 +2652,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>39</v>
       </c>
@@ -2666,7 +2666,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>39</v>
       </c>
@@ -2680,7 +2680,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>39</v>
       </c>
@@ -2694,7 +2694,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>39</v>
       </c>
@@ -2705,7 +2705,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>48</v>
       </c>
@@ -2719,7 +2719,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>48</v>
       </c>
@@ -2733,7 +2733,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>48</v>
       </c>
@@ -2747,7 +2747,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>48</v>
       </c>

</xml_diff>

<commit_message>
added two extra biomarkers to the biomarker_rules_enoc
</commit_message>
<xml_diff>
--- a/inst/extdata/biomarker_rules_enoc.xlsx
+++ b/inst/extdata/biomarker_rules_enoc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hannahokada/Documents/TMAtools/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4DB5EE6-EEA5-1644-BC70-4061F8FFD127}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4B25165-3FFF-DB4C-808B-A59110999D50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14000" yWindow="2340" windowWidth="14800" windowHeight="13100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2680" yWindow="1620" windowWidth="26120" windowHeight="13820" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="translation" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="77">
   <si>
     <t>biomarker</t>
   </si>
@@ -216,6 +216,42 @@
   </si>
   <si>
     <t>absent;reduced</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CD8 </t>
+  </si>
+  <si>
+    <t>CD8</t>
+  </si>
+  <si>
+    <t>1 or 2 IEL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 - 19 IEL </t>
+  </si>
+  <si>
+    <t xml:space="preserve">20 or more IEL </t>
+  </si>
+  <si>
+    <t>Napsin A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">high </t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderate </t>
+  </si>
+  <si>
+    <t>none/low</t>
+  </si>
+  <si>
+    <t xml:space="preserve">else </t>
+  </si>
+  <si>
+    <t>__check__</t>
+  </si>
+  <si>
+    <t>positive</t>
   </si>
 </sst>
 </file>
@@ -603,10 +639,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:C124"/>
+  <dimension ref="A1:C135"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="A77" sqref="A77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1980,6 +2016,127 @@
         <v>32</v>
       </c>
     </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A125" t="s">
+        <v>65</v>
+      </c>
+      <c r="B125" s="5">
+        <v>0</v>
+      </c>
+      <c r="C125" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A126" t="s">
+        <v>65</v>
+      </c>
+      <c r="B126" s="5">
+        <v>1</v>
+      </c>
+      <c r="C126" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A127" t="s">
+        <v>66</v>
+      </c>
+      <c r="B127" s="5">
+        <v>2</v>
+      </c>
+      <c r="C127" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A128" t="s">
+        <v>66</v>
+      </c>
+      <c r="B128" s="5">
+        <v>3</v>
+      </c>
+      <c r="C128" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A129" t="s">
+        <v>66</v>
+      </c>
+      <c r="B129" s="5">
+        <v>9</v>
+      </c>
+      <c r="C129" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A130" t="s">
+        <v>66</v>
+      </c>
+      <c r="B130" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C130" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A131" t="s">
+        <v>70</v>
+      </c>
+      <c r="B131" s="5">
+        <v>0</v>
+      </c>
+      <c r="C131" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A132" t="s">
+        <v>70</v>
+      </c>
+      <c r="B132" s="5">
+        <v>1</v>
+      </c>
+      <c r="C132" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A133" t="s">
+        <v>70</v>
+      </c>
+      <c r="B133" s="5">
+        <v>2</v>
+      </c>
+      <c r="C133" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A134" t="s">
+        <v>70</v>
+      </c>
+      <c r="B134" s="5">
+        <v>9</v>
+      </c>
+      <c r="C134" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A135" t="s">
+        <v>70</v>
+      </c>
+      <c r="B135" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C135" t="s">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1991,10 +2148,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:D57"/>
+  <dimension ref="A1:D68"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="111" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="111" workbookViewId="0">
+      <selection activeCell="G54" sqref="G54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2699,7 +2856,10 @@
         <v>39</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>8</v>
+        <v>5</v>
+      </c>
+      <c r="C53" t="s">
+        <v>56</v>
       </c>
       <c r="D53" t="s">
         <v>56</v>
@@ -2707,44 +2867,41 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C54" t="s">
-        <v>57</v>
+        <v>74</v>
       </c>
       <c r="D54" t="s">
-        <v>57</v>
+        <v>75</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>48</v>
       </c>
-      <c r="B55" s="5">
-        <v>2</v>
+      <c r="B55" s="5" t="s">
+        <v>54</v>
       </c>
       <c r="C55" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D55" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>48</v>
       </c>
-      <c r="B56" s="5" t="s">
-        <v>54</v>
+      <c r="B56" s="5">
+        <v>2</v>
       </c>
       <c r="C56" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="D56" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
@@ -2752,10 +2909,158 @@
         <v>48</v>
       </c>
       <c r="B57" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C57" t="s">
+        <v>51</v>
+      </c>
+      <c r="D57" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>48</v>
+      </c>
+      <c r="B58" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C58" t="s">
+        <v>60</v>
+      </c>
+      <c r="D58" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>48</v>
+      </c>
+      <c r="B59" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D57" t="s">
-        <v>60</v>
+      <c r="D59" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>65</v>
+      </c>
+      <c r="B60" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C60" t="s">
+        <v>69</v>
+      </c>
+      <c r="D60" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>65</v>
+      </c>
+      <c r="B61" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C61" t="s">
+        <v>68</v>
+      </c>
+      <c r="D61" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>66</v>
+      </c>
+      <c r="B62" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C62" t="s">
+        <v>67</v>
+      </c>
+      <c r="D62" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>66</v>
+      </c>
+      <c r="B63" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C63" t="s">
+        <v>56</v>
+      </c>
+      <c r="D63" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>66</v>
+      </c>
+      <c r="B64" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D64" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>70</v>
+      </c>
+      <c r="B65" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C65" t="s">
+        <v>6</v>
+      </c>
+      <c r="D65" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>70</v>
+      </c>
+      <c r="B66" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C66" t="s">
+        <v>7</v>
+      </c>
+      <c r="D66" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>70</v>
+      </c>
+      <c r="B67" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C67" t="s">
+        <v>56</v>
+      </c>
+      <c r="D67" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>70</v>
+      </c>
+      <c r="B68" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D68" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated consolidation rules and error "check"
</commit_message>
<xml_diff>
--- a/inst/extdata/biomarker_rules_enoc.xlsx
+++ b/inst/extdata/biomarker_rules_enoc.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11018"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11102"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hannahokada/Documents/TMAtools/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4B25165-3FFF-DB4C-808B-A59110999D50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FAF3364-879F-4B48-B48B-9AF8614B05C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2680" yWindow="1620" windowWidth="26120" windowHeight="13820" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1180" yWindow="500" windowWidth="27620" windowHeight="15320" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="translation" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="644" uniqueCount="79">
   <si>
     <t>biomarker</t>
   </si>
@@ -53,9 +53,6 @@
     <t>negative</t>
   </si>
   <si>
-    <t>TP53</t>
-  </si>
-  <si>
     <t>Unk</t>
   </si>
   <si>
@@ -252,6 +249,15 @@
   </si>
   <si>
     <t>positive</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wildtype </t>
+  </si>
+  <si>
+    <t xml:space="preserve">present </t>
+  </si>
+  <si>
+    <t xml:space="preserve">reduced </t>
   </si>
 </sst>
 </file>
@@ -641,8 +647,8 @@
   </sheetPr>
   <dimension ref="A1:C135"/>
   <sheetViews>
-    <sheetView topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="A77" sqref="A77"/>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="F48" sqref="F48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -657,10 +663,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -704,7 +710,7 @@
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -712,10 +718,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -723,312 +729,312 @@
         <v>4</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B8" s="4">
         <v>0</v>
       </c>
       <c r="C8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B9" s="4">
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B10" s="4">
         <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B11" s="4">
         <v>3</v>
       </c>
       <c r="C11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B12" s="4">
         <v>4</v>
       </c>
       <c r="C12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B13" s="4">
         <v>5</v>
       </c>
       <c r="C13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B14" s="4">
         <v>8</v>
       </c>
       <c r="C14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B15" s="4">
         <v>9</v>
       </c>
       <c r="C15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B18" s="4">
         <v>0</v>
       </c>
       <c r="C18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B19" s="4">
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20" s="4">
         <v>2</v>
       </c>
       <c r="C20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B21" s="4">
         <v>3</v>
       </c>
       <c r="C21" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B22" s="4">
         <v>8</v>
       </c>
       <c r="C22" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B23" s="4">
         <v>9</v>
       </c>
       <c r="C23" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B24" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C24" t="s">
         <v>31</v>
-      </c>
-      <c r="C24" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C25" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B26" s="4">
         <v>0</v>
       </c>
       <c r="C26" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B27" s="4">
         <v>1</v>
       </c>
       <c r="C27" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B28" s="4">
         <v>2</v>
       </c>
       <c r="C28" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B29" s="4">
         <v>3</v>
       </c>
       <c r="C29" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B30" s="4">
         <v>4</v>
       </c>
       <c r="C30" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B31" s="4">
         <v>5</v>
       </c>
       <c r="C31" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B32" s="4">
         <v>9</v>
       </c>
       <c r="C32" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C33" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C34" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B35" s="4">
         <v>0</v>
@@ -1039,7 +1045,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B36" s="4">
         <v>1</v>
@@ -1050,7 +1056,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B37" s="4">
         <v>2</v>
@@ -1061,40 +1067,40 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B38" s="4">
         <v>9</v>
       </c>
       <c r="C38" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C39" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C40" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B41" s="4">
         <v>0</v>
@@ -1105,7 +1111,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B42" s="4">
         <v>1</v>
@@ -1116,7 +1122,7 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B43" s="4">
         <v>2</v>
@@ -1127,40 +1133,40 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B44" s="4">
         <v>9</v>
       </c>
       <c r="C44" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C45" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C46" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B47" s="4">
         <v>0</v>
@@ -1171,7 +1177,7 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B48" s="4">
         <v>1</v>
@@ -1182,7 +1188,7 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B49" s="4">
         <v>2</v>
@@ -1193,40 +1199,40 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B50" s="4">
         <v>9</v>
       </c>
       <c r="C50" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C51" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C52" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B53" s="4">
         <v>0</v>
@@ -1237,7 +1243,7 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B54" s="4">
         <v>1</v>
@@ -1248,7 +1254,7 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B55" s="4">
         <v>2</v>
@@ -1259,40 +1265,40 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B56" s="4">
         <v>9</v>
       </c>
       <c r="C56" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C57" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C58" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B59" s="4">
         <v>0</v>
@@ -1303,7 +1309,7 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B60" s="4">
         <v>1</v>
@@ -1314,7 +1320,7 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B61" s="4">
         <v>2</v>
@@ -1325,40 +1331,40 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B62" s="4">
         <v>9</v>
       </c>
       <c r="C62" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C63" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C64" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B65" s="4">
         <v>0</v>
@@ -1369,7 +1375,7 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B66" s="4">
         <v>1</v>
@@ -1380,7 +1386,7 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B67" s="4">
         <v>2</v>
@@ -1391,40 +1397,40 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B68" s="4">
         <v>9</v>
       </c>
       <c r="C68" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C69" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C70" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B71" s="5">
         <v>0</v>
@@ -1435,590 +1441,590 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B72" s="5">
         <v>1</v>
       </c>
       <c r="C72" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B73" s="5">
         <v>2</v>
       </c>
       <c r="C73" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B74" s="5">
         <v>3</v>
       </c>
       <c r="C74" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B75" s="5">
         <v>9</v>
       </c>
       <c r="C75" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B76" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C76" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B77" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C77" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B78" s="4">
         <v>0</v>
       </c>
       <c r="C78" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B79" s="4">
         <v>1</v>
       </c>
       <c r="C79" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B80" s="4">
         <v>2</v>
       </c>
       <c r="C80" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B81" s="4">
         <v>3</v>
       </c>
       <c r="C81" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B82" s="4">
         <v>8</v>
       </c>
       <c r="C82" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B83" s="4">
         <v>9</v>
       </c>
       <c r="C83" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C84" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C85" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B86" s="4">
         <v>0</v>
       </c>
       <c r="C86" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B87" s="4">
         <v>1</v>
       </c>
       <c r="C87" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B88" s="4">
         <v>2</v>
       </c>
       <c r="C88" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B89" s="4">
         <v>3</v>
       </c>
       <c r="C89" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B90" s="4">
         <v>8</v>
       </c>
       <c r="C90" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B91" s="4">
         <v>9</v>
       </c>
       <c r="C91" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C92" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C93" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B94" s="4">
         <v>0</v>
       </c>
       <c r="C94" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B95" s="4">
         <v>1</v>
       </c>
       <c r="C95" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B96" s="4">
         <v>2</v>
       </c>
       <c r="C96" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B97" s="4">
         <v>3</v>
       </c>
       <c r="C97" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B98" s="4">
         <v>8</v>
       </c>
       <c r="C98" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B99" s="4">
         <v>9</v>
       </c>
       <c r="C99" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B100" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C100" t="s">
         <v>31</v>
-      </c>
-      <c r="C100" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B101" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C101" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B102" s="4">
         <v>0</v>
       </c>
       <c r="C102" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B103" s="4">
         <v>1</v>
       </c>
       <c r="C103" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B104" s="4">
         <v>2</v>
       </c>
       <c r="C104" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B105" s="4">
         <v>3</v>
       </c>
       <c r="C105" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B106" s="4">
         <v>8</v>
       </c>
       <c r="C106" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B107" s="4">
         <v>9</v>
       </c>
       <c r="C107" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C108" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C109" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B110" s="4">
         <v>0</v>
       </c>
       <c r="C110" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B111" s="4">
         <v>1</v>
       </c>
       <c r="C111" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B112" s="4">
         <v>2</v>
       </c>
       <c r="C112" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B113" s="4">
         <v>3</v>
       </c>
       <c r="C113" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B114" s="4">
         <v>8</v>
       </c>
       <c r="C114" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B115" s="4">
         <v>9</v>
       </c>
       <c r="C115" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C116" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C117" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B118" s="5">
         <v>0</v>
       </c>
       <c r="C118" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B119" s="5">
         <v>1</v>
       </c>
       <c r="C119" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B120" s="5">
         <v>2</v>
       </c>
       <c r="C120" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B121" s="5">
         <v>3</v>
       </c>
       <c r="C121" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B122" s="5">
         <v>9</v>
       </c>
       <c r="C122" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B123" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C123" t="s">
         <v>31</v>
-      </c>
-      <c r="C123" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B124" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C124" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B125" s="5">
         <v>0</v>
@@ -2029,73 +2035,73 @@
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B126" s="5">
         <v>1</v>
       </c>
       <c r="C126" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B127" s="5">
         <v>2</v>
       </c>
       <c r="C127" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B128" s="5">
         <v>3</v>
       </c>
       <c r="C128" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B129" s="5">
         <v>9</v>
       </c>
       <c r="C129" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B130" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C130" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B131" s="5">
         <v>0</v>
       </c>
       <c r="C131" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B132" s="5">
         <v>1</v>
@@ -2106,7 +2112,7 @@
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B133" s="5">
         <v>2</v>
@@ -2117,24 +2123,24 @@
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B134" s="5">
         <v>9</v>
       </c>
       <c r="C134" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B135" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C135" t="s">
         <v>31</v>
-      </c>
-      <c r="C135" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -2148,10 +2154,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:D68"/>
+  <dimension ref="A1:D89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="111" workbookViewId="0">
-      <selection activeCell="G54" sqref="G54"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="111" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2178,7 +2184,7 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>5</v>
@@ -2192,7 +2198,7 @@
     </row>
     <row r="3" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>5</v>
@@ -2206,10 +2212,13 @@
     </row>
     <row r="4" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>8</v>
+        <v>53</v>
+      </c>
+      <c r="C4" t="s">
+        <v>55</v>
       </c>
       <c r="D4" t="s">
         <v>9</v>
@@ -2217,147 +2226,147 @@
     </row>
     <row r="5" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" t="s">
-        <v>12</v>
+        <v>73</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D6" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="D7" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>5</v>
+        <v>53</v>
       </c>
       <c r="C8" t="s">
-        <v>16</v>
+        <v>55</v>
       </c>
       <c r="D8" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" t="s">
-        <v>17</v>
+        <v>73</v>
       </c>
       <c r="D9" t="s">
-        <v>13</v>
+        <v>74</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>61</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
+      </c>
+      <c r="C10" t="s">
+        <v>11</v>
       </c>
       <c r="D10" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>61</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C11" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="D11" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>61</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C12" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="D12" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>61</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
+      </c>
+      <c r="C13" t="s">
+        <v>15</v>
       </c>
       <c r="D13" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>23</v>
+        <v>61</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>54</v>
+        <v>5</v>
       </c>
       <c r="C14" t="s">
-        <v>61</v>
+        <v>16</v>
       </c>
       <c r="D14" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>23</v>
+        <v>61</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>24</v>
+        <v>53</v>
       </c>
       <c r="C15" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="D15" t="s">
         <v>17</v>
@@ -2365,258 +2374,261 @@
     </row>
     <row r="16" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>23</v>
+        <v>61</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C16" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="D16" t="s">
-        <v>17</v>
+        <v>74</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>54</v>
+        <v>5</v>
       </c>
       <c r="C17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C18" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D18" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C19" t="s">
-        <v>26</v>
+        <v>77</v>
       </c>
       <c r="D19" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C20" t="s">
-        <v>27</v>
+        <v>73</v>
       </c>
       <c r="D20" t="s">
-        <v>11</v>
+        <v>74</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C21" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="D21" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
+      </c>
+      <c r="C22" t="s">
+        <v>20</v>
       </c>
       <c r="D22" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>5</v>
+        <v>53</v>
       </c>
       <c r="C23" t="s">
-        <v>6</v>
+        <v>77</v>
       </c>
       <c r="D23" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C24" t="s">
-        <v>7</v>
+        <v>73</v>
       </c>
       <c r="D24" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>22</v>
+      </c>
+      <c r="B25" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B25" s="3" t="s">
-        <v>8</v>
+      <c r="C25" t="s">
+        <v>60</v>
       </c>
       <c r="D25" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="C26" t="s">
-        <v>6</v>
+        <v>63</v>
       </c>
       <c r="D26" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="C27" t="s">
-        <v>7</v>
+        <v>62</v>
       </c>
       <c r="D27" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>8</v>
+        <v>53</v>
+      </c>
+      <c r="C28" t="s">
+        <v>19</v>
       </c>
       <c r="D28" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C29" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="D29" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>5</v>
+        <v>53</v>
       </c>
       <c r="C30" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="D30" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>8</v>
+        <v>53</v>
+      </c>
+      <c r="C31" t="s">
+        <v>26</v>
       </c>
       <c r="D31" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C32" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="D32" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>5</v>
+        <v>53</v>
       </c>
       <c r="C33" t="s">
-        <v>7</v>
+        <v>78</v>
       </c>
       <c r="D33" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>8</v>
+        <v>73</v>
       </c>
       <c r="D34" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>5</v>
@@ -2630,7 +2642,7 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>5</v>
@@ -2644,10 +2656,13 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
+      </c>
+      <c r="C37" t="s">
+        <v>9</v>
       </c>
       <c r="D37" t="s">
         <v>9</v>
@@ -2655,412 +2670,691 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C38" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="D38" t="s">
-        <v>20</v>
+        <v>74</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C39" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="D39" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
+      </c>
+      <c r="C40" t="s">
+        <v>7</v>
       </c>
       <c r="D40" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>5</v>
+        <v>53</v>
       </c>
       <c r="C41" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D41" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C42" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="D42" t="s">
-        <v>20</v>
+        <v>74</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
+      </c>
+      <c r="C43" t="s">
+        <v>6</v>
       </c>
       <c r="D43" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C44" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="D44" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C45" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="D45" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D46" t="s">
-        <v>22</v>
+        <v>74</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C47" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="D47" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C48" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D48" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
+      </c>
+      <c r="C49" t="s">
+        <v>9</v>
       </c>
       <c r="D49" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>39</v>
-      </c>
-      <c r="B50" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C50" t="s">
-        <v>55</v>
+        <v>36</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="D50" t="s">
-        <v>13</v>
+        <v>74</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>39</v>
-      </c>
-      <c r="B51" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B51" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C51" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="D51" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>39</v>
-      </c>
-      <c r="B52" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B52" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C52" t="s">
-        <v>40</v>
+        <v>7</v>
       </c>
       <c r="D52" t="s">
-        <v>40</v>
+        <v>7</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>39</v>
-      </c>
-      <c r="B53" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B53" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C53" t="s">
-        <v>56</v>
+        <v>9</v>
       </c>
       <c r="D53" t="s">
-        <v>56</v>
+        <v>9</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>39</v>
-      </c>
-      <c r="B54" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D54" t="s">
         <v>74</v>
-      </c>
-      <c r="D54" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>48</v>
-      </c>
-      <c r="B55" s="5" t="s">
-        <v>54</v>
+        <v>41</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>5</v>
       </c>
       <c r="C55" t="s">
-        <v>57</v>
+        <v>19</v>
       </c>
       <c r="D55" t="s">
-        <v>57</v>
+        <v>19</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>48</v>
-      </c>
-      <c r="B56" s="5">
-        <v>2</v>
+        <v>41</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>5</v>
       </c>
       <c r="C56" t="s">
-        <v>58</v>
+        <v>20</v>
       </c>
       <c r="D56" t="s">
-        <v>59</v>
+        <v>19</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>48</v>
-      </c>
-      <c r="B57" s="5" t="s">
-        <v>54</v>
+        <v>41</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>5</v>
       </c>
       <c r="C57" t="s">
-        <v>51</v>
+        <v>21</v>
       </c>
       <c r="D57" t="s">
-        <v>51</v>
+        <v>21</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>48</v>
-      </c>
-      <c r="B58" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C58" t="s">
-        <v>60</v>
+        <v>41</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="D58" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>48</v>
-      </c>
-      <c r="B59" s="5" t="s">
-        <v>8</v>
+        <v>44</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C59" t="s">
+        <v>19</v>
       </c>
       <c r="D59" t="s">
-        <v>75</v>
+        <v>19</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>65</v>
-      </c>
-      <c r="B60" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B60" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C60" t="s">
-        <v>69</v>
+        <v>20</v>
       </c>
       <c r="D60" t="s">
-        <v>71</v>
+        <v>19</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>65</v>
-      </c>
-      <c r="B61" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B61" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C61" t="s">
-        <v>68</v>
+        <v>21</v>
       </c>
       <c r="D61" t="s">
-        <v>72</v>
+        <v>21</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>66</v>
-      </c>
-      <c r="B62" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C62" t="s">
-        <v>67</v>
+        <v>44</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="D62" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>66</v>
-      </c>
-      <c r="B63" s="5" t="s">
-        <v>54</v>
+        <v>45</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>5</v>
       </c>
       <c r="C63" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="D63" t="s">
-        <v>73</v>
+        <v>19</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>66</v>
-      </c>
-      <c r="B64" s="5" t="s">
-        <v>74</v>
+        <v>45</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C64" t="s">
+        <v>20</v>
       </c>
       <c r="D64" t="s">
-        <v>75</v>
+        <v>19</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>70</v>
-      </c>
-      <c r="B65" s="5" t="s">
-        <v>54</v>
+        <v>45</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>5</v>
       </c>
       <c r="C65" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="D65" t="s">
-        <v>76</v>
+        <v>21</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>70</v>
-      </c>
-      <c r="B66" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C66" t="s">
-        <v>7</v>
+        <v>45</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="D66" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>70</v>
-      </c>
-      <c r="B67" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B67" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C67" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="D67" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
+        <v>46</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C68" t="s">
+        <v>20</v>
+      </c>
+      <c r="D68" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>46</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C69" t="s">
+        <v>21</v>
+      </c>
+      <c r="D69" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>46</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D70" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>38</v>
+      </c>
+      <c r="B71" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C71" t="s">
+        <v>54</v>
+      </c>
+      <c r="D71" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>38</v>
+      </c>
+      <c r="B72" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C72" t="s">
+        <v>14</v>
+      </c>
+      <c r="D72" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>38</v>
+      </c>
+      <c r="B73" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C73" t="s">
+        <v>39</v>
+      </c>
+      <c r="D73" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>38</v>
+      </c>
+      <c r="B74" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C74" t="s">
+        <v>55</v>
+      </c>
+      <c r="D74" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>38</v>
+      </c>
+      <c r="B75" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="D75" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>47</v>
+      </c>
+      <c r="B76" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C76" t="s">
+        <v>56</v>
+      </c>
+      <c r="D76" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>47</v>
+      </c>
+      <c r="B77" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C77" t="s">
+        <v>57</v>
+      </c>
+      <c r="D77" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>47</v>
+      </c>
+      <c r="B78" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C78" t="s">
+        <v>50</v>
+      </c>
+      <c r="D78" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>47</v>
+      </c>
+      <c r="B79" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C79" t="s">
+        <v>59</v>
+      </c>
+      <c r="D79" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>47</v>
+      </c>
+      <c r="B80" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D80" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>64</v>
+      </c>
+      <c r="B81" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C81" t="s">
+        <v>68</v>
+      </c>
+      <c r="D81" t="s">
         <v>70</v>
       </c>
-      <c r="B68" s="5" t="s">
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>64</v>
+      </c>
+      <c r="B82" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C82" t="s">
+        <v>67</v>
+      </c>
+      <c r="D82" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>65</v>
+      </c>
+      <c r="B83" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C83" t="s">
+        <v>66</v>
+      </c>
+      <c r="D83" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>65</v>
+      </c>
+      <c r="B84" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C84" t="s">
+        <v>55</v>
+      </c>
+      <c r="D84" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>65</v>
+      </c>
+      <c r="B85" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="D85" t="s">
         <v>74</v>
       </c>
-      <c r="D68" t="s">
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>69</v>
+      </c>
+      <c r="B86" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C86" t="s">
+        <v>6</v>
+      </c>
+      <c r="D86" t="s">
         <v>75</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>69</v>
+      </c>
+      <c r="B87" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C87" t="s">
+        <v>7</v>
+      </c>
+      <c r="D87" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>69</v>
+      </c>
+      <c r="B88" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C88" t="s">
+        <v>55</v>
+      </c>
+      <c r="D88" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>69</v>
+      </c>
+      <c r="B89" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="D89" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>